<commit_message>
feat: add 2022-Q3 data
</commit_message>
<xml_diff>
--- a/数据整理/stocks/A股/上证主板/600000-浦发银行.xlsx
+++ b/数据整理/stocks/A股/上证主板/600000-浦发银行.xlsx
@@ -7,13 +7,14 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="总计" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q3" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q2" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q1" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-Q4" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q3" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q4" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q3" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q2" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-Q4" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,14 +489,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2022-Q2</t>
+          <t>2022-Q3</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" t="n">
-        <v>16.93</v>
+        <v>14.85</v>
       </c>
     </row>
     <row r="3">
@@ -504,14 +505,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2022-Q1</t>
+          <t>2022-Q2</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D3" t="n">
-        <v>18.12</v>
+        <v>16.93</v>
       </c>
     </row>
     <row r="4">
@@ -520,14 +521,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2021-Q4</t>
+          <t>2022-Q1</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D4" t="n">
-        <v>19.62</v>
+        <v>18.12</v>
       </c>
     </row>
     <row r="5">
@@ -536,14 +537,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2021-Q3</t>
+          <t>2021-Q4</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D5" t="n">
-        <v>24.23</v>
+        <v>19.62</v>
       </c>
     </row>
     <row r="6">
@@ -552,14 +553,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2021-Q2</t>
+          <t>2021-Q3</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D6" t="n">
-        <v>22.11</v>
+        <v>24.23</v>
       </c>
     </row>
     <row r="7">
@@ -568,14 +569,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2021-Q1</t>
+          <t>2021-Q2</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="D7" t="n">
-        <v>25.68</v>
+        <v>22.11</v>
       </c>
     </row>
     <row r="8">
@@ -584,13 +585,29 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>2021-Q1</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>67</v>
+      </c>
+      <c r="D8" t="n">
+        <v>25.68</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>2020-Q4</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C9" t="n">
         <v>39</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D9" t="n">
         <v>19.24</v>
       </c>
     </row>
@@ -600,6 +617,1504 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>基金代码</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>基金名称</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>基金规模</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>股票总仓位</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>仓位占比</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>持有市值(亿元)</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>仓位排名</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>512800</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>华宝中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>90.69</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>99.00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>3.90</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>3.5369</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>510810</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>汇添富中证上海国企ETF</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>63.53</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>98.46</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>4.98</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>3.1638</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>515290</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>天弘中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>72.25</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>99.65</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>3.92</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2.8322</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>512700</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>南方中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>24.78</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>99.68</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>3.92</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.9714</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>510230</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>国泰上证180金融ETF</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>32.72</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>99.89</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2.74</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0.8965</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>161723</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>招商中证银行指数（LOF）A</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>13.72</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>94.56</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3.71</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.5090</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>161029</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>富国中证银行指数A</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>12.62</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>94.64</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>3.71</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.4682</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>161121</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>易方达中证银行指数（LOF）A</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>11.53</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>94.31</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>3.70</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.4266</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>160631</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>鹏华中证银行指数（LOF）A</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>8.53</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>93.61</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>3.66</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.3122</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>160517</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>博时中证银行指数（LOF）</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>7.74</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>94.76</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>3.72</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.2879</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>515020</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>华夏中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>7.15</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>99.38</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>3.89</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0.2781</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>009860</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>易方达中证银行指数（LOF）C</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>6.65</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>94.31</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>3.70</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0.2460</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>512820</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>汇添富中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4.98</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>99.45</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>3.91</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.1947</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>159887</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>富国中证800银行ETF</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>3.55</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>99.23</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>3.97</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0.1409</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>012042</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>鹏华中证银行指数（LOF）C</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2.08</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>93.61</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>3.66</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0.0761</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>512730</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>鹏华中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1.77</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>95.93</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>3.76</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0.0666</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>516310</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>易方达中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>99.08</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>3.89</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0.0603</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>160418</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>华安中证银行A</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1.56</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>94.53</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>3.71</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0.0579</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>002849</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>金信智能中国2025灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1.09</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>78.83</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>4.10</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>0.0447</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>510130</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>易方达上证中盘ETF</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2.05</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>99.39</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>1.96</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0.0402</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>501310</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>华宝标普沪港深中国增强价值指数（LOF）A</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0.89</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>93.50</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>3.89</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>0.0346</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>515300</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>嘉实沪深300红利低波动ETF</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0.94</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>99.19</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2.85</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>0.0268</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>515280</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>富国中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.64</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>98.83</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>3.88</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>0.0248</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>001413</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>中融鑫起点灵活配置混合A</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.59</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>77.02</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>4.14</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>0.0244</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>516210</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>华安中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.55</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>94.53</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>3.71</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>0.0204</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>011971</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>西藏东财中证银行指数A</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0.42</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>94.96</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>3.73</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>0.0157</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>011972</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>西藏东财中证银行指数C</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>94.96</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>3.73</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>0.0149</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>515500</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>海富通中证长三角领先ETF</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>97.12</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>4.87</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0.0146</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>012221</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>瑞达行业轮动混合A</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>76.17</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>4.29</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0.0129</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>517900</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>招商中证银行AH价格优选ETF</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>96.90</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>4.25</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>0.0128</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>013330</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>富国中证银行指数C</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>94.64</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>3.71</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>0.0104</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>001414</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>中融鑫起点灵活配置混合C</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>77.02</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>4.14</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>0.0087</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>014028</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>招商中证银行指数（LOF）C</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>94.56</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>3.71</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>0.0070</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>012222</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>瑞达行业轮动混合C</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>76.17</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>4.29</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>0.0069</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>014983</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>华安中证银行C</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>94.53</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>3.71</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>0.0045</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>510220</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>华泰柏瑞上证中小盘ETF</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>98.11</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>0.99</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>0.0024</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>007397</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>华宝标普沪港深中国增强价值指数（LOF）C</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>93.50</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>3.89</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>0.0016</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>016343</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>招商中证银行指数（LOF）E</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>94.56</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>3.71</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2061,7 +3576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3105,7 +4620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4263,7 +5778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5991,7 +7506,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -7567,7 +9082,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -10169,7 +11684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
feat: add 2022-Q4 data
</commit_message>
<xml_diff>
--- a/数据整理/stocks/A股/上证主板/600000-浦发银行.xlsx
+++ b/数据整理/stocks/A股/上证主板/600000-浦发银行.xlsx
@@ -7,14 +7,15 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="总计" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q3" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q1" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q4" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q3" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q2" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-Q4" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q4" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-Q1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q4" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q3" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q2" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-Q1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-Q4" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -458,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,14 +490,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2022-Q3</t>
+          <t>2022-Q4</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="n">
-        <v>14.85</v>
+        <v>14.13</v>
       </c>
     </row>
     <row r="3">
@@ -505,14 +506,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2022-Q2</t>
+          <t>2022-Q3</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" t="n">
-        <v>16.93</v>
+        <v>14.85</v>
       </c>
     </row>
     <row r="4">
@@ -521,14 +522,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2022-Q1</t>
+          <t>2022-Q2</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D4" t="n">
-        <v>18.12</v>
+        <v>16.93</v>
       </c>
     </row>
     <row r="5">
@@ -537,14 +538,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2021-Q4</t>
+          <t>2022-Q1</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" t="n">
-        <v>19.62</v>
+        <v>18.12</v>
       </c>
     </row>
     <row r="6">
@@ -553,14 +554,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2021-Q3</t>
+          <t>2021-Q4</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D6" t="n">
-        <v>24.23</v>
+        <v>19.62</v>
       </c>
     </row>
     <row r="7">
@@ -569,14 +570,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2021-Q2</t>
+          <t>2021-Q3</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D7" t="n">
-        <v>22.11</v>
+        <v>24.23</v>
       </c>
     </row>
     <row r="8">
@@ -585,14 +586,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2021-Q1</t>
+          <t>2021-Q2</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="D8" t="n">
-        <v>25.68</v>
+        <v>22.11</v>
       </c>
     </row>
     <row r="9">
@@ -601,14 +602,1568 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>2021-Q1</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>67</v>
+      </c>
+      <c r="D9" t="n">
+        <v>25.68</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>2020-Q4</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>39</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>19.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>基金代码</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>基金名称</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>基金金额</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>股票总仓位</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>仓位占比</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>持有市值(亿元)</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>仓位排名</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>510810</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>汇添富中证上海国企ETF</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>101.40</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>97.87</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>6.05</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>6.1347</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>512800</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>华宝中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>92.31</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>99.05</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>4.92</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>4.5417</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>008895</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>申万菱信量化对冲策略灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8.60</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>56.17</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>21.20</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1.8232</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>160631</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>鹏华中证银行指数（LOF）</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>30.15</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>94.12</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>4.67</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1.4080</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>510230</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>国泰上证180金融ETF</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>49.25</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>99.85</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2.78</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1.3692</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>512700</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>南方中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>17.50</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>99.75</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>4.95</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.8662</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>161723</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>招商中证银行指数（LOF）</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>12.60</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>94.21</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>4.64</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.5846</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>161121</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>易方达中证银行指数（LOF）A</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>8.03</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>94.53</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>4.68</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.3758</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>161029</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>富国中证银行指数</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>6.33</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>92.68</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>4.60</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.2912</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>160418</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>华安中证银行指数（LOF）A</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>5.24</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>94.81</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>4.68</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.2452</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>512820</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>汇添富中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>4.51</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>99.55</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>4.95</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0.2232</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>160517</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>博时中证银行指数（LOF）</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>3.79</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>94.06</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>4.64</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0.1759</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>009860</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>易方达中证银行指数（LOF）C</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>3.69</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>94.53</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>4.68</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.1727</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>515020</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>华夏中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>3.04</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>98.14</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>4.93</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0.1499</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>165521</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>信诚中证800金融指数（LOF）</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>5.65</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>94.96</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0.1130</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>004818</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>国寿安保目标策略灵活配置混合A</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>5.73</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>36.67</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0.0968</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>515500</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>海富通中证长三角领先ETF</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2.22</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>94.64</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>4.30</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0.0955</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>512730</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>鹏华中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>97.02</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>4.79</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0.0742</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>450008</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>国富沪深300指数增强</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>4.07</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>92.85</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>1.74</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>0.0708</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>005870</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>鹏华沪深300指数增强</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>3.11</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>93.17</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2.26</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0.0703</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>002849</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>金信智能中国2025灵活配置混合</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0.97</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>85.33</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>6.19</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>0.0600</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>519677</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>银河定投宝中证腾讯济安价值100A股指数</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>93.30</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>1.37</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>0.0401</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>510030</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>华宝上证180价值ETF</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>1.23</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>99.57</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2.64</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>0.0325</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>501060</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>中金中证优选300指数（LOF）A</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>1.78</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>94.90</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>0.0312</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>009096</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>鹏华安泽混合A</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>3.12</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>28.44</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>0.98</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>0.0306</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>510650</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>华夏金融ETF</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0.76</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>97.81</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>3.20</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>0.0243</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>515280</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>富国中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>96.57</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>4.82</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>0.0217</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>168205</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>中融中证银行指数（LOF）</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>92.77</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>4.57</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0.0206</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>510090</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>建信上证社会责任ETF</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.86</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>97.08</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2.24</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0.0193</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>004819</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>国寿安保目标策略灵活配置混合C</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>1.05</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>36.67</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>0.0177</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>510690</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>兴业上证180金融ETF</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0.62</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>98.52</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>0.0170</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>004484</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>泰达宏利业绩驱动量化股票A</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0.84</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>94.04</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2.01</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>0.0169</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>006698</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>红土创新沪深300指数增强A</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>94.48</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>3.35</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>0.0157</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>006699</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>红土创新沪深300指数增强C</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>94.48</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>3.35</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>0.0050</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>006349</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>中金MSCI中国A股国际价值指数A</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>95.04</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2.42</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>0.0039</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>501061</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>中金中证优选300指数（LOF）C</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>94.90</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>0.0018</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>006350</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>中金MSCI中国A股国际价值指数C</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>95.04</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2.42</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>0.0005</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>004485</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>泰达宏利业绩驱动量化股票C</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>94.04</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2.01</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>0.0004</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>009097</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>鹏华安泽混合C</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>28.44</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>0.98</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>0.0003</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -617,6 +2172,1466 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>基金代码</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>基金名称</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>基金规模</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>股票总仓位</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>仓位占比</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>持有市值(亿元)</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>仓位排名</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>510810</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>汇添富中证上海国企ETF</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>65.67</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>98.06</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>4.88</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>3.2047</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>512800</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>华宝中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>74.57</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>98.98</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>3.75</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2.7964</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>515290</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>天弘中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>63.51</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>99.91</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>3.79</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2.4070</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>510230</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>国泰上证180金融ETF</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>35.19</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>99.85</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2.72</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.9572</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>512700</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>南方中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>22.33</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>99.97</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>3.79</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0.8463</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>016343</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>招商中证银行指数（LOF）E</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>13.85</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>94.91</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3.59</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.4972</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>161723</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>招商中证银行指数（LOF）A</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>13.67</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>94.91</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>3.59</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.4908</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>161029</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>富国中证银行指数A</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>13.28</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>94.60</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>3.59</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.4768</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>161121</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>易方达中证银行指数（LOF）A</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>12.13</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>94.37</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>3.58</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0.4343</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>160631</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>鹏华中证银行指数（LOF）A</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>8.19</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>94.59</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>3.58</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.2932</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>160517</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>博时中证银行指数（LOF）</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>7.62</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>94.73</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>3.59</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0.2736</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>515020</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>华夏中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5.87</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>99.29</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>3.75</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0.2201</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>009860</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>易方达中证银行指数（LOF）C</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>6.11</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>94.37</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>3.58</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.2187</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>512820</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>汇添富中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>5.15</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>99.41</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>3.77</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0.1942</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>561300</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>国泰沪深300增强策略ETF</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>11.40</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>96.37</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>1.52</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0.1733</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>159887</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>富国中证800银行ETF</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3.45</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>99.55</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>3.95</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0.1363</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>012042</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>鹏华中证银行指数（LOF）C</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2.21</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>94.59</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>3.58</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0.0791</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>160418</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>华安中证银行A</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2.12</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>94.43</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>3.58</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0.0759</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>512730</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>鹏华中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>98.16</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>3.71</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>0.0668</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>516310</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>易方达中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>98.89</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>3.75</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0.0574</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>510130</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>易方达上证中盘ETF</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>99.08</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>1.94</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>0.0427</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>501310</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>华宝标普沪港深中国增强价值指数（LOF）A</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0.96</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>94.81</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>3.81</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>0.0366</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>001413</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>中融鑫起点灵活配置混合A</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>53.65</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>4.38</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>0.0263</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>515280</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>富国中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.61</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>99.24</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>3.76</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>0.0229</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>012221</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>瑞达行业轮动混合A</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.44</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>75.49</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>4.24</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>0.0187</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>516210</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>华安中证银行ETF</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0.51</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>94.43</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>3.58</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>0.0183</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>517900</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>招商中证银行AH价格优选ETF</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0.43</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>98.38</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>3.65</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>0.0157</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>011971</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>西藏东财中证银行指数A</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0.42</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>94.96</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>3.60</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0.0151</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>007924</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>方正富邦天鑫灵活配置混合C</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>45.12</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2.90</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0.0130</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>011972</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>西藏东财中证银行指数C</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0.33</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>94.96</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>3.60</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>0.0119</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>013330</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>富国中证银行指数C</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>94.60</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>3.59</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>0.0079</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>001414</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>中融鑫起点灵活配置混合C</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>53.65</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>4.38</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>0.0079</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>014028</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>招商中证银行指数（LOF）C</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>94.91</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>3.59</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>0.0061</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>012222</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>瑞达行业轮动混合C</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>75.49</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>4.24</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>0.0034</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>007397</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>华宝标普沪港深中国增强价值指数（LOF）C</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>94.81</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>3.81</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>0.0027</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>007923</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>方正富邦天鑫灵活配置混合A</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>45.12</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2.90</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>014983</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>华安中证银行C</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>-0.42</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>94.43</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>3.58</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-0.0150</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2114,7 +5129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3576,7 +6591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4620,7 +7635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5778,7 +8793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -7506,7 +10521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -9082,7 +12097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -11682,1542 +14697,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>基金代码</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>基金名称</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>基金金额</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>股票总仓位</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>仓位占比</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>持有市值(亿元)</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>仓位排名</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>510810</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>汇添富中证上海国企ETF</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>101.40</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>97.87</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>6.05</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>6.1347</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>512800</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>华宝中证银行ETF</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>92.31</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>99.05</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>4.92</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>4.5417</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>008895</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>申万菱信量化对冲策略灵活配置混合</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>8.60</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>56.17</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>21.20</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>1.8232</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>160631</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>鹏华中证银行指数（LOF）</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>30.15</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>94.12</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>4.67</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>1.4080</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>510230</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>国泰上证180金融ETF</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>49.25</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>99.85</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2.78</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>1.3692</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>512700</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>南方中证银行ETF</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>17.50</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>99.75</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>4.95</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>0.8662</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>161723</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>招商中证银行指数（LOF）</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>12.60</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>94.21</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>4.64</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>0.5846</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>161121</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>易方达中证银行指数（LOF）A</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>8.03</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>94.53</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>4.68</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>0.3758</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>161029</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>富国中证银行指数</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>6.33</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>92.68</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>4.60</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0.2912</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>160418</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>华安中证银行指数（LOF）A</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>5.24</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>94.81</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>4.68</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>0.2452</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>512820</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>汇添富中证银行ETF</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>4.51</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>99.55</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>4.95</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>0.2232</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>160517</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>博时中证银行指数（LOF）</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>3.79</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>94.06</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>4.64</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>0.1759</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>009860</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>易方达中证银行指数（LOF）C</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>3.69</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>94.53</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>4.68</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>0.1727</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>515020</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>华夏中证银行ETF</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>3.04</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>98.14</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>4.93</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>0.1499</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>165521</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>信诚中证800金融指数（LOF）</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>5.65</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>94.96</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2.00</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>0.1130</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>004818</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>国寿安保目标策略灵活配置混合A</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>5.73</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>36.67</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>1.69</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>0.0968</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>515500</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>海富通中证长三角领先ETF</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2.22</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>94.64</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>4.30</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>0.0955</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>512730</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>鹏华中证银行ETF</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>1.55</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>97.02</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>4.79</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>0.0742</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>450008</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>国富沪深300指数增强</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>4.07</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>92.85</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>1.74</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>0.0708</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>005870</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>鹏华沪深300指数增强</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>3.11</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>93.17</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2.26</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>0.0703</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>002849</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>金信智能中国2025灵活配置混合</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>0.97</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>85.33</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>6.19</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>0.0600</t>
-        </is>
-      </c>
-      <c r="H22" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>519677</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>银河定投宝中证腾讯济安价值100A股指数</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>2.93</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>93.30</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>1.37</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>0.0401</t>
-        </is>
-      </c>
-      <c r="H23" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>510030</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>华宝上证180价值ETF</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>1.23</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>99.57</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>2.64</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>0.0325</t>
-        </is>
-      </c>
-      <c r="H24" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>501060</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>中金中证优选300指数（LOF）A</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>1.78</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>94.90</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>1.75</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>0.0312</t>
-        </is>
-      </c>
-      <c r="H25" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>009096</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>鹏华安泽混合A</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>3.12</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>28.44</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>0.98</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>0.0306</t>
-        </is>
-      </c>
-      <c r="H26" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>510650</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>华夏金融ETF</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>0.76</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>97.81</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>3.20</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>0.0243</t>
-        </is>
-      </c>
-      <c r="H27" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>515280</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>富国中证银行ETF</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>0.45</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>96.57</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>4.82</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>0.0217</t>
-        </is>
-      </c>
-      <c r="H28" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>168205</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>中融中证银行指数（LOF）</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>0.45</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>92.77</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>4.57</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>0.0206</t>
-        </is>
-      </c>
-      <c r="H29" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>510090</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>建信上证社会责任ETF</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>0.86</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>97.08</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>2.24</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>0.0193</t>
-        </is>
-      </c>
-      <c r="H30" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>004819</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>国寿安保目标策略灵活配置混合C</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>1.05</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>36.67</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>1.69</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>0.0177</t>
-        </is>
-      </c>
-      <c r="H31" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>510690</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>兴业上证180金融ETF</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>0.62</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>98.52</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>2.75</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>0.0170</t>
-        </is>
-      </c>
-      <c r="H32" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>004484</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>泰达宏利业绩驱动量化股票A</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>0.84</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>94.04</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>2.01</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>0.0169</t>
-        </is>
-      </c>
-      <c r="H33" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>006698</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>红土创新沪深300指数增强A</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>0.47</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>94.48</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>3.35</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>0.0157</t>
-        </is>
-      </c>
-      <c r="H34" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>006699</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>红土创新沪深300指数增强C</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>0.15</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>94.48</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>3.35</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>0.0050</t>
-        </is>
-      </c>
-      <c r="H35" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>006349</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>中金MSCI中国A股国际价值指数A</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>95.04</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>2.42</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>0.0039</t>
-        </is>
-      </c>
-      <c r="H36" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="2" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>501061</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>中金中证优选300指数（LOF）C</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>0.10</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>94.90</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>1.75</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>0.0018</t>
-        </is>
-      </c>
-      <c r="H37" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="2" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>006350</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>中金MSCI中国A股国际价值指数C</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>95.04</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>2.42</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>0.0005</t>
-        </is>
-      </c>
-      <c r="H38" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="2" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>004485</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>泰达宏利业绩驱动量化股票C</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>94.04</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>2.01</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>0.0004</t>
-        </is>
-      </c>
-      <c r="H39" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="2" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>009097</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>鹏华安泽混合C</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>0.03</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>28.44</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>0.98</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>0.0003</t>
-        </is>
-      </c>
-      <c r="H40" t="n">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>